<commit_message>
BOM finished, Sourcing merged
</commit_message>
<xml_diff>
--- a/Group_7_BillOfMaterials.xlsx
+++ b/Group_7_BillOfMaterials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba8bb3ba8fa52c85/Dokumente/TUT/Embedded Systems and Electronics Productization/Project/MySynth_ELT-23056/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{E0E17C42-9361-4E12-8144-DB50785EE3F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0BC7A69A-D4BB-4045-8922-EEB1EAB11F0D}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{E0E17C42-9361-4E12-8144-DB50785EE3F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1BD3A5A4-2419-405A-BDD2-47285E8ACBC6}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" xr2:uid="{37C27555-DE82-4D13-9DBD-47ABDEE1FB9C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -63,16 +63,23 @@
   </si>
   <si>
     <t>n/A</t>
+  </si>
+  <si>
+    <t>PIFACE CONTROL &amp; DISPLAY 2</t>
+  </si>
+  <si>
+    <t>https://fi.farnell.com/piface/piface-control-display-2/i-o-board-w-lcd-for-raspberry/dp/2434231?st=raspberry%20display</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +91,14 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,14 +142,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -144,8 +160,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D74BA9B-4170-4732-8AB5-8CCED1788405}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A9" sqref="A9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +549,30 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>26.49</v>
+      </c>
+      <c r="D8">
+        <v>2434231</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="3"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E8" r:id="rId1" xr:uid="{D17B0657-2226-4D12-A547-B0B19B11F82D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Risk Managmeent added, BOM updated
</commit_message>
<xml_diff>
--- a/Group_7_BillOfMaterials.xlsx
+++ b/Group_7_BillOfMaterials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba8bb3ba8fa52c85/Dokumente/TUT/Embedded Systems and Electronics Productization/Project/MySynth_ELT-23056/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{E0E17C42-9361-4E12-8144-DB50785EE3F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1BD3A5A4-2419-405A-BDD2-47285E8ACBC6}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{E0E17C42-9361-4E12-8144-DB50785EE3F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F03C13F3-FBEB-4AFC-B9CA-6A829EBFD367}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" xr2:uid="{37C27555-DE82-4D13-9DBD-47ABDEE1FB9C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -69,6 +69,39 @@
   </si>
   <si>
     <t>https://fi.farnell.com/piface/piface-control-display-2/i-o-board-w-lcd-for-raspberry/dp/2434231?st=raspberry%20display</t>
+  </si>
+  <si>
+    <t>https://fi.farnell.com/molex/68784-0003/micro-usb-cable-assembly/dp/2125830?st=micro%20usb%20cable</t>
+  </si>
+  <si>
+    <t>4,33€</t>
+  </si>
+  <si>
+    <t>Micro USB Cable</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/USB-Soundkarte-2-0-AM-stereo/dp/B0015QQWPK</t>
+  </si>
+  <si>
+    <t>ALTERNATIVE: USB Soundkarte 2.0 USB AM - 2x3,5mm stereo Buchse [PC]</t>
+  </si>
+  <si>
+    <t>8,94€</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/Stecker-Mikrofon-Buchse-Adapter-Konverter-Klinke-wei%C3%9F/dp/B00PHAPW56</t>
+  </si>
+  <si>
+    <t>ALTERNATIVE: USB A Stecker auf 2 x 3,5 mm Kopf/Mikrofon-Buchse Adapter/Konverter Kabel – AUX Klinke</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>TUTLAB</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -79,7 +112,7 @@
     <numFmt numFmtId="164" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +135,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -146,11 +185,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -160,8 +198,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -477,35 +530,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D74BA9B-4170-4732-8AB5-8CCED1788405}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:E9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="11"/>
     <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="85.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="1"/>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="12" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -516,63 +570,131 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="9">
         <v>56</v>
       </c>
       <c r="D6">
         <v>2894857</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="9">
         <v>12</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>11</v>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10">
         <v>26.49</v>
       </c>
-      <c r="D8">
+      <c r="D10">
         <v>2434231</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E10" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="3"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="7">
+        <v>2125830</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1" xr:uid="{D17B0657-2226-4D12-A547-B0B19B11F82D}"/>
+    <hyperlink ref="E10" r:id="rId1" xr:uid="{D17B0657-2226-4D12-A547-B0B19B11F82D}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{F4B4B681-D5C2-428B-AEEF-90541E1C55F6}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{A4D0F037-7698-434B-906D-8CE54FA5F4CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>